<commit_message>
Mudado valores validados nas telas
</commit_message>
<xml_diff>
--- a/cypress/downloads/Conciliação Bancária .xlsx
+++ b/cypress/downloads/Conciliação Bancária .xlsx
@@ -80,15 +80,15 @@
     <t>21177</t>
   </si>
   <si>
+    <t>Bradesco</t>
+  </si>
+  <si>
+    <t>105546</t>
+  </si>
+  <si>
     <t>Sem domicílio bancário</t>
   </si>
   <si>
-    <t>Bradesco</t>
-  </si>
-  <si>
-    <t>105546</t>
-  </si>
-  <si>
     <t>11364</t>
   </si>
   <si>
@@ -107,16 +107,16 @@
     <t>371.607,36</t>
   </si>
   <si>
-    <t>-1.903,96</t>
-  </si>
-  <si>
-    <t>369.703,40</t>
+    <t>-897,17</t>
+  </si>
+  <si>
+    <t>370.710,19</t>
   </si>
   <si>
     <t>0,00</t>
   </si>
   <si>
-    <t>-369.703,40</t>
+    <t>-370.710,19</t>
   </si>
 </sst>
 </file>
@@ -614,34 +614,38 @@
       </c>
     </row>
     <row r="12" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s"/>
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="3" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D12" s="5" t="n">
         <v>45174</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>45289.216516203705</v>
+        <v>45427.52137731481</v>
       </c>
       <c r="F12" s="7" t="n">
-        <v>0</v>
+        <v>348.15</v>
       </c>
       <c r="G12" s="7" t="n">
-        <v>-536.7</v>
+        <v>-6.76</v>
       </c>
       <c r="H12" s="7" t="n">
-        <v>-536.7</v>
+        <v>341.39</v>
       </c>
       <c r="I12" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J12" s="7" t="n">
-        <v>536.7</v>
+        <v>-341.39</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -652,28 +656,28 @@
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>45174</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>45289.216516203705</v>
+        <v>45427.52137731481</v>
       </c>
       <c r="F13" s="7" t="n">
-        <v>348.15</v>
+        <v>1584.63</v>
       </c>
       <c r="G13" s="7" t="n">
-        <v>-6.76</v>
+        <v>-205.02</v>
       </c>
       <c r="H13" s="7" t="n">
-        <v>341.39</v>
+        <v>1379.61</v>
       </c>
       <c r="I13" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J13" s="7" t="n">
-        <v>-341.39</v>
+        <v>-1379.61</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>13</v>
@@ -681,34 +685,34 @@
     </row>
     <row r="14" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4" t="n">
-        <v>1</v>
+        <v>237</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5" t="n">
         <v>45174</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>45289.216516203705</v>
+        <v>45427.52137731481</v>
       </c>
       <c r="F14" s="7" t="n">
-        <v>1584.63</v>
+        <v>14463.73</v>
       </c>
       <c r="G14" s="7" t="n">
-        <v>-205.02</v>
+        <v>0</v>
       </c>
       <c r="H14" s="7" t="n">
-        <v>1379.61</v>
+        <v>14463.73</v>
       </c>
       <c r="I14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J14" s="7" t="n">
-        <v>-1379.61</v>
+        <v>-14463.73</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>13</v>
@@ -716,80 +720,80 @@
     </row>
     <row r="15" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4" t="n">
-        <v>237</v>
+        <v>748</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>45174</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>45289.216516203705</v>
+        <v>45427.52137731481</v>
       </c>
       <c r="F15" s="7" t="n">
-        <v>14463.73</v>
+        <v>5054.76</v>
       </c>
       <c r="G15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="7" t="n">
-        <v>14463.73</v>
+        <v>5054.76</v>
       </c>
       <c r="I15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J15" s="7" t="n">
-        <v>-14463.73</v>
+        <v>-5054.76</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16" s="3" t="s"/>
       <c r="B16" s="4" t="n">
-        <v>748</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s"/>
       <c r="D16" s="5" t="n">
-        <v>45174</v>
+        <v>45175</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>45289.216516203705</v>
+        <v>45176.74318287037</v>
       </c>
       <c r="F16" s="7" t="n">
-        <v>5054.76</v>
+        <v>0</v>
       </c>
       <c r="G16" s="7" t="n">
-        <v>0</v>
+        <v>-58.86</v>
       </c>
       <c r="H16" s="7" t="n">
-        <v>5054.76</v>
+        <v>-58.86</v>
       </c>
       <c r="I16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J16" s="7" t="n">
-        <v>-5054.76</v>
+        <v>58.86</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s"/>
+      <c r="A17" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D17" s="5" t="n">
         <v>45175</v>
       </c>
@@ -797,22 +801,22 @@
         <v>45176.74318287037</v>
       </c>
       <c r="F17" s="7" t="n">
-        <v>0</v>
+        <v>1483.75</v>
       </c>
       <c r="G17" s="7" t="n">
-        <v>-58.86</v>
+        <v>0</v>
       </c>
       <c r="H17" s="7" t="n">
-        <v>-58.86</v>
+        <v>1483.75</v>
       </c>
       <c r="I17" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J17" s="7" t="n">
-        <v>58.86</v>
+        <v>-1483.75</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -823,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>45175</v>
@@ -832,19 +836,19 @@
         <v>45176.74318287037</v>
       </c>
       <c r="F18" s="7" t="n">
-        <v>1483.75</v>
+        <v>941.23</v>
       </c>
       <c r="G18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="7" t="n">
-        <v>1483.75</v>
+        <v>941.23</v>
       </c>
       <c r="I18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J18" s="7" t="n">
-        <v>-1483.75</v>
+        <v>-941.23</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>13</v>
@@ -858,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>45175</v>
@@ -867,19 +871,19 @@
         <v>45176.74318287037</v>
       </c>
       <c r="F19" s="7" t="n">
-        <v>941.23</v>
+        <v>2653.08</v>
       </c>
       <c r="G19" s="7" t="n">
-        <v>0</v>
+        <v>-201.8</v>
       </c>
       <c r="H19" s="7" t="n">
-        <v>941.23</v>
+        <v>2451.28</v>
       </c>
       <c r="I19" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J19" s="7" t="n">
-        <v>-941.23</v>
+        <v>-2451.28</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>13</v>
@@ -887,13 +891,13 @@
     </row>
     <row r="20" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="n">
-        <v>1</v>
+        <v>341</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D20" s="5" t="n">
         <v>45175</v>
@@ -902,19 +906,19 @@
         <v>45176.74318287037</v>
       </c>
       <c r="F20" s="7" t="n">
-        <v>2653.08</v>
+        <v>142.7</v>
       </c>
       <c r="G20" s="7" t="n">
-        <v>-201.8</v>
+        <v>0</v>
       </c>
       <c r="H20" s="7" t="n">
-        <v>2451.28</v>
+        <v>142.7</v>
       </c>
       <c r="I20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="7" t="n">
-        <v>-2451.28</v>
+        <v>-142.7</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>13</v>
@@ -922,13 +926,13 @@
     </row>
     <row r="21" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4" t="n">
-        <v>341</v>
+        <v>748</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>45175</v>
@@ -937,19 +941,19 @@
         <v>45176.74318287037</v>
       </c>
       <c r="F21" s="7" t="n">
-        <v>142.7</v>
+        <v>3575.46</v>
       </c>
       <c r="G21" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="7" t="n">
-        <v>142.7</v>
+        <v>3575.46</v>
       </c>
       <c r="I21" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="7" t="n">
-        <v>-142.7</v>
+        <v>-3575.46</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>13</v>
@@ -966,25 +970,25 @@
         <v>17</v>
       </c>
       <c r="D22" s="5" t="n">
-        <v>45175</v>
+        <v>45176</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>45176.74318287037</v>
+        <v>45177.56060185185</v>
       </c>
       <c r="F22" s="7" t="n">
-        <v>3575.46</v>
+        <v>490.84</v>
       </c>
       <c r="G22" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="7" t="n">
-        <v>3575.46</v>
+        <v>490.84</v>
       </c>
       <c r="I22" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="7" t="n">
-        <v>-3575.46</v>
+        <v>-490.84</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>13</v>
@@ -992,34 +996,34 @@
     </row>
     <row r="23" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B23" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>45176</v>
+        <v>45177</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>45177.56060185185</v>
+        <v>45178.70140046296</v>
       </c>
       <c r="F23" s="7" t="n">
-        <v>490.84</v>
+        <v>264.14</v>
       </c>
       <c r="G23" s="7" t="n">
-        <v>0</v>
+        <v>-8.03</v>
       </c>
       <c r="H23" s="7" t="n">
-        <v>490.84</v>
+        <v>256.11</v>
       </c>
       <c r="I23" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J23" s="7" t="n">
-        <v>-490.84</v>
+        <v>-256.11</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>13</v>
@@ -1033,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>45177</v>
@@ -1042,19 +1046,19 @@
         <v>45178.70140046296</v>
       </c>
       <c r="F24" s="7" t="n">
-        <v>264.14</v>
+        <v>1862.52</v>
       </c>
       <c r="G24" s="7" t="n">
         <v>-8.03</v>
       </c>
       <c r="H24" s="7" t="n">
-        <v>256.11</v>
+        <v>1854.49</v>
       </c>
       <c r="I24" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="7" t="n">
-        <v>-256.11</v>
+        <v>-1854.49</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>13</v>
@@ -1068,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>45177</v>
@@ -1077,19 +1081,19 @@
         <v>45178.70140046296</v>
       </c>
       <c r="F25" s="7" t="n">
-        <v>1862.52</v>
+        <v>5513.64</v>
       </c>
       <c r="G25" s="7" t="n">
-        <v>-8.03</v>
+        <v>0</v>
       </c>
       <c r="H25" s="7" t="n">
-        <v>1854.49</v>
+        <v>5513.64</v>
       </c>
       <c r="I25" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="7" t="n">
-        <v>-1854.49</v>
+        <v>-5513.64</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>13</v>
@@ -1097,13 +1101,13 @@
     </row>
     <row r="26" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B26" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>45177</v>
@@ -1112,19 +1116,19 @@
         <v>45178.70140046296</v>
       </c>
       <c r="F26" s="7" t="n">
-        <v>5513.64</v>
+        <v>9586.06</v>
       </c>
       <c r="G26" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="7" t="n">
-        <v>5513.64</v>
+        <v>9586.06</v>
       </c>
       <c r="I26" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="7" t="n">
-        <v>-5513.64</v>
+        <v>-9586.06</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>13</v>
@@ -1141,25 +1145,25 @@
         <v>17</v>
       </c>
       <c r="D27" s="5" t="n">
-        <v>45177</v>
+        <v>45178</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>45178.70140046296</v>
+        <v>45179.484085648146</v>
       </c>
       <c r="F27" s="7" t="n">
-        <v>9586.06</v>
+        <v>433.76</v>
       </c>
       <c r="G27" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="7" t="n">
-        <v>9586.06</v>
+        <v>433.76</v>
       </c>
       <c r="I27" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="7" t="n">
-        <v>-9586.06</v>
+        <v>-433.76</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>13</v>
@@ -1176,25 +1180,25 @@
         <v>17</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>45178</v>
+        <v>45179</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>45179.484085648146</v>
+        <v>45180.64466435185</v>
       </c>
       <c r="F28" s="7" t="n">
-        <v>433.76</v>
+        <v>211.3</v>
       </c>
       <c r="G28" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="7" t="n">
-        <v>433.76</v>
+        <v>211.3</v>
       </c>
       <c r="I28" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J28" s="7" t="n">
-        <v>-433.76</v>
+        <v>-211.3</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>13</v>
@@ -1202,34 +1206,34 @@
     </row>
     <row r="29" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B29" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D29" s="5" t="n">
-        <v>45179</v>
+        <v>45180</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>45180.64466435185</v>
+        <v>45251.85450231482</v>
       </c>
       <c r="F29" s="7" t="n">
-        <v>211.3</v>
+        <v>10206.06</v>
       </c>
       <c r="G29" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H29" s="7" t="n">
-        <v>211.3</v>
+        <v>10206.06</v>
       </c>
       <c r="I29" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J29" s="7" t="n">
-        <v>-211.3</v>
+        <v>-10206.06</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>13</v>
@@ -1237,13 +1241,13 @@
     </row>
     <row r="30" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B30" s="4" t="n">
-        <v>1</v>
+        <v>341</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>45180</v>
@@ -1252,19 +1256,19 @@
         <v>45251.85450231482</v>
       </c>
       <c r="F30" s="7" t="n">
-        <v>10206.06</v>
+        <v>5520.45</v>
       </c>
       <c r="G30" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H30" s="7" t="n">
-        <v>10206.06</v>
+        <v>5520.45</v>
       </c>
       <c r="I30" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J30" s="7" t="n">
-        <v>-10206.06</v>
+        <v>-5520.45</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>13</v>
@@ -1272,13 +1276,13 @@
     </row>
     <row r="31" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B31" s="4" t="n">
-        <v>341</v>
+        <v>748</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>45180</v>
@@ -1287,19 +1291,19 @@
         <v>45251.85450231482</v>
       </c>
       <c r="F31" s="7" t="n">
-        <v>5520.45</v>
+        <v>9371.26</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>0</v>
+        <v>-116.7</v>
       </c>
       <c r="H31" s="7" t="n">
-        <v>5520.45</v>
+        <v>9254.56</v>
       </c>
       <c r="I31" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J31" s="7" t="n">
-        <v>-5520.45</v>
+        <v>-9254.56</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>13</v>
@@ -1307,146 +1311,150 @@
     </row>
     <row r="32" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="5" t="n">
+        <v>45181</v>
+      </c>
+      <c r="E32" s="6" t="n">
+        <v>45427.52439814815</v>
+      </c>
+      <c r="F32" s="7" t="n">
+        <v>1478.24</v>
+      </c>
+      <c r="G32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7" t="n">
+        <v>1478.24</v>
+      </c>
+      <c r="I32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="7" t="n">
+        <v>-1478.24</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="4" t="n">
+      <c r="B33" s="4" t="n">
         <v>748</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="5" t="n">
-        <v>45180</v>
-      </c>
-      <c r="E32" s="6" t="n">
-        <v>45251.85450231482</v>
-      </c>
-      <c r="F32" s="7" t="n">
-        <v>9371.26</v>
-      </c>
-      <c r="G32" s="7" t="n">
-        <v>-116.7</v>
-      </c>
-      <c r="H32" s="7" t="n">
-        <v>9254.56</v>
-      </c>
-      <c r="I32" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" s="7" t="n">
-        <v>-9254.56</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s"/>
-      <c r="B33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3" t="s"/>
       <c r="D33" s="5" t="n">
         <v>45181</v>
       </c>
       <c r="E33" s="6" t="n">
-        <v>45289.21488425926</v>
+        <v>45427.52439814815</v>
       </c>
       <c r="F33" s="7" t="n">
-        <v>0</v>
+        <v>4935.51</v>
       </c>
       <c r="G33" s="7" t="n">
-        <v>-213.6</v>
+        <v>0</v>
       </c>
       <c r="H33" s="7" t="n">
-        <v>-213.6</v>
+        <v>4935.51</v>
       </c>
       <c r="I33" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J33" s="7" t="n">
-        <v>213.6</v>
+        <v>-4935.51</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A34" s="3" t="s"/>
       <c r="B34" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="s"/>
       <c r="D34" s="5" t="n">
-        <v>45181</v>
+        <v>45182</v>
       </c>
       <c r="E34" s="6" t="n">
-        <v>45289.21488425926</v>
+        <v>45183.766064814816</v>
       </c>
       <c r="F34" s="7" t="n">
-        <v>1478.24</v>
+        <v>0</v>
       </c>
       <c r="G34" s="7" t="n">
-        <v>0</v>
+        <v>-1.04</v>
       </c>
       <c r="H34" s="7" t="n">
-        <v>1478.24</v>
+        <v>-1.04</v>
       </c>
       <c r="I34" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J34" s="7" t="n">
-        <v>-1478.24</v>
+        <v>1.04</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B35" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>45181</v>
+        <v>45182</v>
       </c>
       <c r="E35" s="6" t="n">
-        <v>45289.21488425926</v>
+        <v>45183.766064814816</v>
       </c>
       <c r="F35" s="7" t="n">
-        <v>4935.51</v>
+        <v>1.46</v>
       </c>
       <c r="G35" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H35" s="7" t="n">
-        <v>4935.51</v>
+        <v>1.46</v>
       </c>
       <c r="I35" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J35" s="7" t="n">
-        <v>-4935.51</v>
+        <v>-1.46</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s"/>
+      <c r="A36" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D36" s="5" t="n">
         <v>45182</v>
       </c>
@@ -1454,33 +1462,33 @@
         <v>45183.766064814816</v>
       </c>
       <c r="F36" s="7" t="n">
-        <v>0</v>
+        <v>2463.99</v>
       </c>
       <c r="G36" s="7" t="n">
-        <v>-1.04</v>
+        <v>0</v>
       </c>
       <c r="H36" s="7" t="n">
-        <v>-1.04</v>
+        <v>2463.99</v>
       </c>
       <c r="I36" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J36" s="7" t="n">
-        <v>1.04</v>
+        <v>-2463.99</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B37" s="4" t="n">
-        <v>1</v>
+        <v>341</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>45182</v>
@@ -1489,19 +1497,19 @@
         <v>45183.766064814816</v>
       </c>
       <c r="F37" s="7" t="n">
-        <v>1.46</v>
+        <v>150.64</v>
       </c>
       <c r="G37" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H37" s="7" t="n">
-        <v>1.46</v>
+        <v>150.64</v>
       </c>
       <c r="I37" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J37" s="7" t="n">
-        <v>-1.46</v>
+        <v>-150.64</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>13</v>
@@ -1509,13 +1517,13 @@
     </row>
     <row r="38" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B38" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>45182</v>
@@ -1524,19 +1532,19 @@
         <v>45183.766064814816</v>
       </c>
       <c r="F38" s="7" t="n">
-        <v>2463.99</v>
+        <v>3130.77</v>
       </c>
       <c r="G38" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="7" t="n">
-        <v>2463.99</v>
+        <v>3130.77</v>
       </c>
       <c r="I38" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J38" s="7" t="n">
-        <v>-2463.99</v>
+        <v>-3130.77</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>13</v>
@@ -1544,34 +1552,34 @@
     </row>
     <row r="39" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B39" s="4" t="n">
-        <v>341</v>
+        <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D39" s="5" t="n">
-        <v>45182</v>
+        <v>45183</v>
       </c>
       <c r="E39" s="6" t="n">
-        <v>45183.766064814816</v>
+        <v>45184.52064814815</v>
       </c>
       <c r="F39" s="7" t="n">
-        <v>150.64</v>
+        <v>4202.99</v>
       </c>
       <c r="G39" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H39" s="7" t="n">
-        <v>150.64</v>
+        <v>4202.99</v>
       </c>
       <c r="I39" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J39" s="7" t="n">
-        <v>-150.64</v>
+        <v>-4202.99</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>13</v>
@@ -1588,25 +1596,25 @@
         <v>17</v>
       </c>
       <c r="D40" s="5" t="n">
-        <v>45182</v>
+        <v>45183</v>
       </c>
       <c r="E40" s="6" t="n">
-        <v>45183.766064814816</v>
+        <v>45184.52064814815</v>
       </c>
       <c r="F40" s="7" t="n">
-        <v>3130.77</v>
+        <v>3148.01</v>
       </c>
       <c r="G40" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H40" s="7" t="n">
-        <v>3130.77</v>
+        <v>3148.01</v>
       </c>
       <c r="I40" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J40" s="7" t="n">
-        <v>-3130.77</v>
+        <v>-3148.01</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>13</v>
@@ -1620,28 +1628,28 @@
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D41" s="5" t="n">
-        <v>45183</v>
+        <v>45184</v>
       </c>
       <c r="E41" s="6" t="n">
-        <v>45184.52064814815</v>
+        <v>45187.50225694444</v>
       </c>
       <c r="F41" s="7" t="n">
-        <v>4202.99</v>
+        <v>483.51</v>
       </c>
       <c r="G41" s="7" t="n">
-        <v>0</v>
+        <v>-8.03</v>
       </c>
       <c r="H41" s="7" t="n">
-        <v>4202.99</v>
+        <v>475.48</v>
       </c>
       <c r="I41" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J41" s="7" t="n">
-        <v>-4202.99</v>
+        <v>-475.48</v>
       </c>
       <c r="K41" s="3" t="s">
         <v>13</v>
@@ -1649,34 +1657,34 @@
     </row>
     <row r="42" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B42" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>45183</v>
+        <v>45184</v>
       </c>
       <c r="E42" s="6" t="n">
-        <v>45184.52064814815</v>
+        <v>45187.50225694444</v>
       </c>
       <c r="F42" s="7" t="n">
-        <v>3148.01</v>
+        <v>949.91</v>
       </c>
       <c r="G42" s="7" t="n">
-        <v>0</v>
+        <v>-16.06</v>
       </c>
       <c r="H42" s="7" t="n">
-        <v>3148.01</v>
+        <v>933.85</v>
       </c>
       <c r="I42" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J42" s="7" t="n">
-        <v>-3148.01</v>
+        <v>-933.85</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>13</v>
@@ -1690,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D43" s="5" t="n">
         <v>45184</v>
@@ -1699,19 +1707,19 @@
         <v>45187.50225694444</v>
       </c>
       <c r="F43" s="7" t="n">
-        <v>483.51</v>
+        <v>4560.23</v>
       </c>
       <c r="G43" s="7" t="n">
-        <v>-8.03</v>
+        <v>0</v>
       </c>
       <c r="H43" s="7" t="n">
-        <v>475.48</v>
+        <v>4560.23</v>
       </c>
       <c r="I43" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J43" s="7" t="n">
-        <v>-475.48</v>
+        <v>-4560.23</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>13</v>
@@ -1719,13 +1727,13 @@
     </row>
     <row r="44" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B44" s="4" t="n">
-        <v>1</v>
+        <v>341</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D44" s="5" t="n">
         <v>45184</v>
@@ -1734,19 +1742,19 @@
         <v>45187.50225694444</v>
       </c>
       <c r="F44" s="7" t="n">
-        <v>949.91</v>
+        <v>17.38</v>
       </c>
       <c r="G44" s="7" t="n">
-        <v>-16.06</v>
+        <v>0</v>
       </c>
       <c r="H44" s="7" t="n">
-        <v>933.85</v>
+        <v>17.38</v>
       </c>
       <c r="I44" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J44" s="7" t="n">
-        <v>-933.85</v>
+        <v>-17.38</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>13</v>
@@ -1754,13 +1762,13 @@
     </row>
     <row r="45" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B45" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D45" s="5" t="n">
         <v>45184</v>
@@ -1769,19 +1777,19 @@
         <v>45187.50225694444</v>
       </c>
       <c r="F45" s="7" t="n">
-        <v>4560.23</v>
+        <v>2225.75</v>
       </c>
       <c r="G45" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H45" s="7" t="n">
-        <v>4560.23</v>
+        <v>2225.75</v>
       </c>
       <c r="I45" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J45" s="7" t="n">
-        <v>-4560.23</v>
+        <v>-2225.75</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>13</v>
@@ -1789,34 +1797,34 @@
     </row>
     <row r="46" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B46" s="4" t="n">
-        <v>341</v>
+        <v>748</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D46" s="5" t="n">
-        <v>45184</v>
+        <v>45185</v>
       </c>
       <c r="E46" s="6" t="n">
-        <v>45187.50225694444</v>
+        <v>45186.475752314815</v>
       </c>
       <c r="F46" s="7" t="n">
-        <v>17.38</v>
+        <v>117.24</v>
       </c>
       <c r="G46" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H46" s="7" t="n">
-        <v>17.38</v>
+        <v>117.24</v>
       </c>
       <c r="I46" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J46" s="7" t="n">
-        <v>-17.38</v>
+        <v>-117.24</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>13</v>
@@ -1833,25 +1841,25 @@
         <v>17</v>
       </c>
       <c r="D47" s="5" t="n">
-        <v>45184</v>
+        <v>45186</v>
       </c>
       <c r="E47" s="6" t="n">
-        <v>45187.50225694444</v>
+        <v>45187.572534722225</v>
       </c>
       <c r="F47" s="7" t="n">
-        <v>2225.75</v>
+        <v>158.82</v>
       </c>
       <c r="G47" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H47" s="7" t="n">
-        <v>2225.75</v>
+        <v>158.82</v>
       </c>
       <c r="I47" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J47" s="7" t="n">
-        <v>-2225.75</v>
+        <v>-158.82</v>
       </c>
       <c r="K47" s="3" t="s">
         <v>13</v>
@@ -1859,34 +1867,34 @@
     </row>
     <row r="48" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B48" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D48" s="5" t="n">
-        <v>45185</v>
+        <v>45187</v>
       </c>
       <c r="E48" s="6" t="n">
-        <v>45186.475752314815</v>
+        <v>45280.33611111111</v>
       </c>
       <c r="F48" s="7" t="n">
-        <v>117.24</v>
+        <v>69.65</v>
       </c>
       <c r="G48" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H48" s="7" t="n">
-        <v>117.24</v>
+        <v>69.65</v>
       </c>
       <c r="I48" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J48" s="7" t="n">
-        <v>-117.24</v>
+        <v>-69.65</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>13</v>
@@ -1894,34 +1902,34 @@
     </row>
     <row r="49" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B49" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D49" s="5" t="n">
-        <v>45186</v>
+        <v>45187</v>
       </c>
       <c r="E49" s="6" t="n">
-        <v>45187.572534722225</v>
+        <v>45280.33611111111</v>
       </c>
       <c r="F49" s="7" t="n">
-        <v>158.82</v>
+        <v>92.53</v>
       </c>
       <c r="G49" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H49" s="7" t="n">
-        <v>158.82</v>
+        <v>92.53</v>
       </c>
       <c r="I49" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J49" s="7" t="n">
-        <v>-158.82</v>
+        <v>-92.53</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>13</v>
@@ -1935,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D50" s="5" t="n">
         <v>45187</v>
@@ -1944,19 +1952,19 @@
         <v>45280.33611111111</v>
       </c>
       <c r="F50" s="7" t="n">
-        <v>69.65</v>
+        <v>5304.2</v>
       </c>
       <c r="G50" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="7" t="n">
-        <v>69.65</v>
+        <v>5304.2</v>
       </c>
       <c r="I50" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J50" s="7" t="n">
-        <v>-69.65</v>
+        <v>-5304.2</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>13</v>
@@ -1964,13 +1972,13 @@
     </row>
     <row r="51" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B51" s="4" t="n">
-        <v>1</v>
+        <v>341</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>45187</v>
@@ -1979,19 +1987,19 @@
         <v>45280.33611111111</v>
       </c>
       <c r="F51" s="7" t="n">
-        <v>92.53</v>
+        <v>4214.39</v>
       </c>
       <c r="G51" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H51" s="7" t="n">
-        <v>92.53</v>
+        <v>4214.39</v>
       </c>
       <c r="I51" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J51" s="7" t="n">
-        <v>-92.53</v>
+        <v>-4214.39</v>
       </c>
       <c r="K51" s="3" t="s">
         <v>13</v>
@@ -1999,13 +2007,13 @@
     </row>
     <row r="52" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B52" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D52" s="5" t="n">
         <v>45187</v>
@@ -2014,19 +2022,19 @@
         <v>45280.33611111111</v>
       </c>
       <c r="F52" s="7" t="n">
-        <v>5304.2</v>
+        <v>7205.6</v>
       </c>
       <c r="G52" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H52" s="7" t="n">
-        <v>5304.2</v>
+        <v>7205.6</v>
       </c>
       <c r="I52" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J52" s="7" t="n">
-        <v>-5304.2</v>
+        <v>-7205.6</v>
       </c>
       <c r="K52" s="3" t="s">
         <v>13</v>
@@ -2034,34 +2042,34 @@
     </row>
     <row r="53" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B53" s="4" t="n">
-        <v>341</v>
+        <v>1</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D53" s="5" t="n">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="E53" s="6" t="n">
-        <v>45280.33611111111</v>
+        <v>45427.534583333334</v>
       </c>
       <c r="F53" s="7" t="n">
-        <v>4214.39</v>
+        <v>2080.68</v>
       </c>
       <c r="G53" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H53" s="7" t="n">
-        <v>4214.39</v>
+        <v>2080.68</v>
       </c>
       <c r="I53" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J53" s="7" t="n">
-        <v>-4214.39</v>
+        <v>-2080.68</v>
       </c>
       <c r="K53" s="3" t="s">
         <v>13</v>
@@ -2069,135 +2077,135 @@
     </row>
     <row r="54" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="4" t="n">
+        <v>237</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="5" t="n">
+        <v>45188</v>
+      </c>
+      <c r="E54" s="6" t="n">
+        <v>45427.534583333334</v>
+      </c>
+      <c r="F54" s="7" t="n">
+        <v>22900.82</v>
+      </c>
+      <c r="G54" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="7" t="n">
+        <v>22900.82</v>
+      </c>
+      <c r="I54" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" s="7" t="n">
+        <v>-22900.82</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="4" t="n">
+      <c r="B55" s="4" t="n">
         <v>748</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="5" t="n">
-        <v>45187</v>
-      </c>
-      <c r="E54" s="6" t="n">
-        <v>45280.33611111111</v>
-      </c>
-      <c r="F54" s="7" t="n">
-        <v>7205.6</v>
-      </c>
-      <c r="G54" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" s="7" t="n">
-        <v>7205.6</v>
-      </c>
-      <c r="I54" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J54" s="7" t="n">
-        <v>-7205.6</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s"/>
-      <c r="B55" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C55" s="3" t="s"/>
       <c r="D55" s="5" t="n">
         <v>45188</v>
       </c>
       <c r="E55" s="6" t="n">
-        <v>45356.83547453704</v>
+        <v>45427.534583333334</v>
       </c>
       <c r="F55" s="7" t="n">
-        <v>0</v>
+        <v>2141.67</v>
       </c>
       <c r="G55" s="7" t="n">
-        <v>-173.58</v>
+        <v>0</v>
       </c>
       <c r="H55" s="7" t="n">
-        <v>-173.58</v>
+        <v>2141.67</v>
       </c>
       <c r="I55" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J55" s="7" t="n">
-        <v>173.58</v>
+        <v>-2141.67</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A56" s="3" t="s"/>
       <c r="B56" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C56" s="3" t="s"/>
       <c r="D56" s="5" t="n">
-        <v>45188</v>
+        <v>45189</v>
       </c>
       <c r="E56" s="6" t="n">
-        <v>45356.83547453704</v>
+        <v>45190.71706018518</v>
       </c>
       <c r="F56" s="7" t="n">
-        <v>2080.68</v>
+        <v>0</v>
       </c>
       <c r="G56" s="7" t="n">
-        <v>0</v>
+        <v>-4.47</v>
       </c>
       <c r="H56" s="7" t="n">
-        <v>2080.68</v>
+        <v>-4.47</v>
       </c>
       <c r="I56" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J56" s="7" t="n">
-        <v>-2080.68</v>
+        <v>4.47</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B57" s="4" t="n">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D57" s="5" t="n">
-        <v>45188</v>
+        <v>45189</v>
       </c>
       <c r="E57" s="6" t="n">
-        <v>45356.83547453704</v>
+        <v>45190.71706018518</v>
       </c>
       <c r="F57" s="7" t="n">
-        <v>22900.82</v>
+        <v>23145.85</v>
       </c>
       <c r="G57" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H57" s="7" t="n">
-        <v>22900.82</v>
+        <v>23145.85</v>
       </c>
       <c r="I57" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J57" s="7" t="n">
-        <v>-22900.82</v>
+        <v>-23145.85</v>
       </c>
       <c r="K57" s="3" t="s">
         <v>13</v>
@@ -2205,45 +2213,49 @@
     </row>
     <row r="58" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B58" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D58" s="5" t="n">
-        <v>45188</v>
+        <v>45189</v>
       </c>
       <c r="E58" s="6" t="n">
-        <v>45356.83547453704</v>
+        <v>45190.71706018518</v>
       </c>
       <c r="F58" s="7" t="n">
-        <v>2141.67</v>
+        <v>642.85</v>
       </c>
       <c r="G58" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H58" s="7" t="n">
-        <v>2141.67</v>
+        <v>642.85</v>
       </c>
       <c r="I58" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J58" s="7" t="n">
-        <v>-2141.67</v>
+        <v>-642.85</v>
       </c>
       <c r="K58" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s"/>
+      <c r="A59" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B59" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C59" s="3" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D59" s="5" t="n">
         <v>45189</v>
       </c>
@@ -2251,33 +2263,33 @@
         <v>45190.71706018518</v>
       </c>
       <c r="F59" s="7" t="n">
-        <v>0</v>
+        <v>2288.34</v>
       </c>
       <c r="G59" s="7" t="n">
-        <v>-4.47</v>
+        <v>0</v>
       </c>
       <c r="H59" s="7" t="n">
-        <v>-4.47</v>
+        <v>2288.34</v>
       </c>
       <c r="I59" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J59" s="7" t="n">
-        <v>4.47</v>
+        <v>-2288.34</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B60" s="4" t="n">
-        <v>1</v>
+        <v>341</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D60" s="5" t="n">
         <v>45189</v>
@@ -2286,19 +2298,19 @@
         <v>45190.71706018518</v>
       </c>
       <c r="F60" s="7" t="n">
-        <v>23145.85</v>
+        <v>9850.37</v>
       </c>
       <c r="G60" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H60" s="7" t="n">
-        <v>23145.85</v>
+        <v>9850.37</v>
       </c>
       <c r="I60" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J60" s="7" t="n">
-        <v>-23145.85</v>
+        <v>-9850.37</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>13</v>
@@ -2306,13 +2318,13 @@
     </row>
     <row r="61" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B61" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D61" s="5" t="n">
         <v>45189</v>
@@ -2321,19 +2333,19 @@
         <v>45190.71706018518</v>
       </c>
       <c r="F61" s="7" t="n">
-        <v>642.85</v>
+        <v>2576.06</v>
       </c>
       <c r="G61" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H61" s="7" t="n">
-        <v>642.85</v>
+        <v>2576.06</v>
       </c>
       <c r="I61" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J61" s="7" t="n">
-        <v>-642.85</v>
+        <v>-2576.06</v>
       </c>
       <c r="K61" s="3" t="s">
         <v>13</v>
@@ -2347,28 +2359,28 @@
         <v>1</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D62" s="5" t="n">
-        <v>45189</v>
+        <v>45190</v>
       </c>
       <c r="E62" s="6" t="n">
-        <v>45190.71706018518</v>
+        <v>45344.105416666665</v>
       </c>
       <c r="F62" s="7" t="n">
-        <v>2288.34</v>
+        <v>504.74</v>
       </c>
       <c r="G62" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H62" s="7" t="n">
-        <v>2288.34</v>
+        <v>504.74</v>
       </c>
       <c r="I62" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J62" s="7" t="n">
-        <v>-2288.34</v>
+        <v>-504.74</v>
       </c>
       <c r="K62" s="3" t="s">
         <v>13</v>
@@ -2376,34 +2388,34 @@
     </row>
     <row r="63" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B63" s="4" t="n">
-        <v>341</v>
+        <v>1</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D63" s="5" t="n">
-        <v>45189</v>
+        <v>45190</v>
       </c>
       <c r="E63" s="6" t="n">
-        <v>45190.71706018518</v>
+        <v>45344.105416666665</v>
       </c>
       <c r="F63" s="7" t="n">
-        <v>9850.37</v>
+        <v>4536.2</v>
       </c>
       <c r="G63" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H63" s="7" t="n">
-        <v>9850.37</v>
+        <v>4536.2</v>
       </c>
       <c r="I63" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J63" s="7" t="n">
-        <v>-9850.37</v>
+        <v>-4536.2</v>
       </c>
       <c r="K63" s="3" t="s">
         <v>13</v>
@@ -2411,34 +2423,34 @@
     </row>
     <row r="64" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B64" s="4" t="n">
-        <v>748</v>
+        <v>341</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D64" s="5" t="n">
-        <v>45189</v>
+        <v>45190</v>
       </c>
       <c r="E64" s="6" t="n">
-        <v>45190.71706018518</v>
+        <v>45344.105416666665</v>
       </c>
       <c r="F64" s="7" t="n">
-        <v>2576.06</v>
+        <v>109.44</v>
       </c>
       <c r="G64" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H64" s="7" t="n">
-        <v>2576.06</v>
+        <v>109.44</v>
       </c>
       <c r="I64" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J64" s="7" t="n">
-        <v>-2576.06</v>
+        <v>-109.44</v>
       </c>
       <c r="K64" s="3" t="s">
         <v>13</v>
@@ -2446,13 +2458,13 @@
     </row>
     <row r="65" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B65" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D65" s="5" t="n">
         <v>45190</v>
@@ -2461,19 +2473,19 @@
         <v>45344.105416666665</v>
       </c>
       <c r="F65" s="7" t="n">
-        <v>504.74</v>
+        <v>2531.46</v>
       </c>
       <c r="G65" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H65" s="7" t="n">
-        <v>504.74</v>
+        <v>2531.46</v>
       </c>
       <c r="I65" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J65" s="7" t="n">
-        <v>-504.74</v>
+        <v>-2531.46</v>
       </c>
       <c r="K65" s="3" t="s">
         <v>13</v>
@@ -2487,28 +2499,28 @@
         <v>1</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D66" s="5" t="n">
-        <v>45190</v>
+        <v>45191</v>
       </c>
       <c r="E66" s="6" t="n">
-        <v>45344.105416666665</v>
+        <v>45192.56958333333</v>
       </c>
       <c r="F66" s="7" t="n">
-        <v>4536.2</v>
+        <v>679.19</v>
       </c>
       <c r="G66" s="7" t="n">
-        <v>0</v>
+        <v>-16.06</v>
       </c>
       <c r="H66" s="7" t="n">
-        <v>4536.2</v>
+        <v>663.13</v>
       </c>
       <c r="I66" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J66" s="7" t="n">
-        <v>-4536.2</v>
+        <v>-663.13</v>
       </c>
       <c r="K66" s="3" t="s">
         <v>13</v>
@@ -2516,34 +2528,34 @@
     </row>
     <row r="67" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B67" s="4" t="n">
-        <v>341</v>
+        <v>1</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D67" s="5" t="n">
-        <v>45190</v>
+        <v>45191</v>
       </c>
       <c r="E67" s="6" t="n">
-        <v>45344.105416666665</v>
+        <v>45192.56958333333</v>
       </c>
       <c r="F67" s="7" t="n">
-        <v>109.44</v>
+        <v>3067.26</v>
       </c>
       <c r="G67" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H67" s="7" t="n">
-        <v>109.44</v>
+        <v>3067.26</v>
       </c>
       <c r="I67" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J67" s="7" t="n">
-        <v>-109.44</v>
+        <v>-3067.26</v>
       </c>
       <c r="K67" s="3" t="s">
         <v>13</v>
@@ -2560,25 +2572,25 @@
         <v>17</v>
       </c>
       <c r="D68" s="5" t="n">
-        <v>45190</v>
+        <v>45191</v>
       </c>
       <c r="E68" s="6" t="n">
-        <v>45344.105416666665</v>
+        <v>45192.56958333333</v>
       </c>
       <c r="F68" s="7" t="n">
-        <v>2531.46</v>
+        <v>3273.92</v>
       </c>
       <c r="G68" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H68" s="7" t="n">
-        <v>2531.46</v>
+        <v>3273.92</v>
       </c>
       <c r="I68" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J68" s="7" t="n">
-        <v>-2531.46</v>
+        <v>-3273.92</v>
       </c>
       <c r="K68" s="3" t="s">
         <v>13</v>
@@ -2586,34 +2598,34 @@
     </row>
     <row r="69" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B69" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D69" s="5" t="n">
-        <v>45191</v>
+        <v>45192</v>
       </c>
       <c r="E69" s="6" t="n">
-        <v>45192.56958333333</v>
+        <v>45193.424212962964</v>
       </c>
       <c r="F69" s="7" t="n">
-        <v>679.19</v>
+        <v>141.49</v>
       </c>
       <c r="G69" s="7" t="n">
-        <v>-16.06</v>
+        <v>0</v>
       </c>
       <c r="H69" s="7" t="n">
-        <v>663.13</v>
+        <v>141.49</v>
       </c>
       <c r="I69" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J69" s="7" t="n">
-        <v>-663.13</v>
+        <v>-141.49</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>13</v>
@@ -2627,28 +2639,28 @@
         <v>1</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D70" s="5" t="n">
-        <v>45191</v>
+        <v>45194</v>
       </c>
       <c r="E70" s="6" t="n">
-        <v>45192.56958333333</v>
+        <v>45196.063252314816</v>
       </c>
       <c r="F70" s="7" t="n">
-        <v>3067.26</v>
+        <v>187.4</v>
       </c>
       <c r="G70" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H70" s="7" t="n">
-        <v>3067.26</v>
+        <v>187.4</v>
       </c>
       <c r="I70" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J70" s="7" t="n">
-        <v>-3067.26</v>
+        <v>-187.4</v>
       </c>
       <c r="K70" s="3" t="s">
         <v>13</v>
@@ -2656,34 +2668,34 @@
     </row>
     <row r="71" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B71" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D71" s="5" t="n">
-        <v>45191</v>
+        <v>45194</v>
       </c>
       <c r="E71" s="6" t="n">
-        <v>45192.56958333333</v>
+        <v>45196.063252314816</v>
       </c>
       <c r="F71" s="7" t="n">
-        <v>3273.92</v>
+        <v>57.26</v>
       </c>
       <c r="G71" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H71" s="7" t="n">
-        <v>3273.92</v>
+        <v>57.26</v>
       </c>
       <c r="I71" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J71" s="7" t="n">
-        <v>-3273.92</v>
+        <v>-57.26</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>13</v>
@@ -2691,34 +2703,34 @@
     </row>
     <row r="72" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B72" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D72" s="5" t="n">
-        <v>45192</v>
+        <v>45194</v>
       </c>
       <c r="E72" s="6" t="n">
-        <v>45193.424212962964</v>
+        <v>45196.063252314816</v>
       </c>
       <c r="F72" s="7" t="n">
-        <v>141.49</v>
+        <v>9452.83</v>
       </c>
       <c r="G72" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H72" s="7" t="n">
-        <v>141.49</v>
+        <v>9452.83</v>
       </c>
       <c r="I72" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J72" s="7" t="n">
-        <v>-141.49</v>
+        <v>-9452.83</v>
       </c>
       <c r="K72" s="3" t="s">
         <v>13</v>
@@ -2726,13 +2738,13 @@
     </row>
     <row r="73" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B73" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D73" s="5" t="n">
         <v>45194</v>
@@ -2741,19 +2753,19 @@
         <v>45196.063252314816</v>
       </c>
       <c r="F73" s="7" t="n">
-        <v>187.4</v>
+        <v>6451.64</v>
       </c>
       <c r="G73" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H73" s="7" t="n">
-        <v>187.4</v>
+        <v>6451.64</v>
       </c>
       <c r="I73" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J73" s="7" t="n">
-        <v>-187.4</v>
+        <v>-6451.64</v>
       </c>
       <c r="K73" s="3" t="s">
         <v>13</v>
@@ -2767,28 +2779,28 @@
         <v>1</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D74" s="5" t="n">
-        <v>45194</v>
+        <v>45195</v>
       </c>
       <c r="E74" s="6" t="n">
-        <v>45196.063252314816</v>
+        <v>45427.54880787037</v>
       </c>
       <c r="F74" s="7" t="n">
-        <v>57.26</v>
+        <v>640.99</v>
       </c>
       <c r="G74" s="7" t="n">
-        <v>0</v>
+        <v>-211.8</v>
       </c>
       <c r="H74" s="7" t="n">
-        <v>57.26</v>
+        <v>429.19</v>
       </c>
       <c r="I74" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J74" s="7" t="n">
-        <v>-57.26</v>
+        <v>-429.19</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>13</v>
@@ -2805,25 +2817,25 @@
         <v>15</v>
       </c>
       <c r="D75" s="5" t="n">
-        <v>45194</v>
+        <v>45195</v>
       </c>
       <c r="E75" s="6" t="n">
-        <v>45196.063252314816</v>
+        <v>45427.54880787037</v>
       </c>
       <c r="F75" s="7" t="n">
-        <v>9452.83</v>
+        <v>4948.24</v>
       </c>
       <c r="G75" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H75" s="7" t="n">
-        <v>9452.83</v>
+        <v>4948.24</v>
       </c>
       <c r="I75" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J75" s="7" t="n">
-        <v>-9452.83</v>
+        <v>-4948.24</v>
       </c>
       <c r="K75" s="3" t="s">
         <v>13</v>
@@ -2831,103 +2843,103 @@
     </row>
     <row r="76" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B76" s="4" t="n">
+        <v>237</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" s="5" t="n">
+        <v>45195</v>
+      </c>
+      <c r="E76" s="6" t="n">
+        <v>45427.54880787037</v>
+      </c>
+      <c r="F76" s="7" t="n">
+        <v>26754.25</v>
+      </c>
+      <c r="G76" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" s="7" t="n">
+        <v>26754.25</v>
+      </c>
+      <c r="I76" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" s="7" t="n">
+        <v>-26754.25</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B76" s="4" t="n">
+      <c r="B77" s="4" t="n">
         <v>748</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D76" s="5" t="n">
-        <v>45194</v>
-      </c>
-      <c r="E76" s="6" t="n">
-        <v>45196.063252314816</v>
-      </c>
-      <c r="F76" s="7" t="n">
-        <v>6451.64</v>
-      </c>
-      <c r="G76" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H76" s="7" t="n">
-        <v>6451.64</v>
-      </c>
-      <c r="I76" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J76" s="7" t="n">
-        <v>-6451.64</v>
-      </c>
-      <c r="K76" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s"/>
-      <c r="B77" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C77" s="3" t="s"/>
       <c r="D77" s="5" t="n">
         <v>45195</v>
       </c>
       <c r="E77" s="6" t="n">
-        <v>45289.21637731481</v>
+        <v>45427.54880787037</v>
       </c>
       <c r="F77" s="7" t="n">
-        <v>0</v>
+        <v>4159.25</v>
       </c>
       <c r="G77" s="7" t="n">
-        <v>-82.91</v>
+        <v>0</v>
       </c>
       <c r="H77" s="7" t="n">
-        <v>-82.91</v>
+        <v>4159.25</v>
       </c>
       <c r="I77" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J77" s="7" t="n">
-        <v>82.91</v>
+        <v>-4159.25</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A78" s="3" t="s"/>
       <c r="B78" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C78" s="3" t="s"/>
       <c r="D78" s="5" t="n">
-        <v>45195</v>
+        <v>45196</v>
       </c>
       <c r="E78" s="6" t="n">
-        <v>45289.21637731481</v>
+        <v>45197.75108796296</v>
       </c>
       <c r="F78" s="7" t="n">
-        <v>640.99</v>
+        <v>0</v>
       </c>
       <c r="G78" s="7" t="n">
-        <v>-211.8</v>
+        <v>-2.39</v>
       </c>
       <c r="H78" s="7" t="n">
-        <v>429.19</v>
+        <v>-2.39</v>
       </c>
       <c r="I78" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J78" s="7" t="n">
-        <v>-429.19</v>
+        <v>2.39</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -2938,28 +2950,28 @@
         <v>1</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D79" s="5" t="n">
-        <v>45195</v>
+        <v>45196</v>
       </c>
       <c r="E79" s="6" t="n">
-        <v>45289.21637731481</v>
+        <v>45197.75108796296</v>
       </c>
       <c r="F79" s="7" t="n">
-        <v>4948.24</v>
+        <v>46.92</v>
       </c>
       <c r="G79" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H79" s="7" t="n">
-        <v>4948.24</v>
+        <v>46.92</v>
       </c>
       <c r="I79" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J79" s="7" t="n">
-        <v>-4948.24</v>
+        <v>-46.92</v>
       </c>
       <c r="K79" s="3" t="s">
         <v>13</v>
@@ -2967,34 +2979,34 @@
     </row>
     <row r="80" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B80" s="4" t="n">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D80" s="5" t="n">
-        <v>45195</v>
+        <v>45196</v>
       </c>
       <c r="E80" s="6" t="n">
-        <v>45289.21637731481</v>
+        <v>45197.75108796296</v>
       </c>
       <c r="F80" s="7" t="n">
-        <v>26754.25</v>
+        <v>2746.16</v>
       </c>
       <c r="G80" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H80" s="7" t="n">
-        <v>26754.25</v>
+        <v>2746.16</v>
       </c>
       <c r="I80" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J80" s="7" t="n">
-        <v>-26754.25</v>
+        <v>-2746.16</v>
       </c>
       <c r="K80" s="3" t="s">
         <v>13</v>
@@ -3011,91 +3023,95 @@
         <v>17</v>
       </c>
       <c r="D81" s="5" t="n">
-        <v>45195</v>
+        <v>45196</v>
       </c>
       <c r="E81" s="6" t="n">
-        <v>45289.21637731481</v>
+        <v>45197.75108796296</v>
       </c>
       <c r="F81" s="7" t="n">
-        <v>4159.25</v>
+        <v>13968.83</v>
       </c>
       <c r="G81" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H81" s="7" t="n">
-        <v>4159.25</v>
+        <v>13968.83</v>
       </c>
       <c r="I81" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J81" s="7" t="n">
-        <v>-4159.25</v>
+        <v>-13968.83</v>
       </c>
       <c r="K81" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s"/>
+      <c r="A82" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B82" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C82" s="3" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D82" s="5" t="n">
-        <v>45196</v>
+        <v>45197</v>
       </c>
       <c r="E82" s="6" t="n">
-        <v>45197.75108796296</v>
+        <v>45197.403645833336</v>
       </c>
       <c r="F82" s="7" t="n">
-        <v>0</v>
+        <v>1553.39</v>
       </c>
       <c r="G82" s="7" t="n">
-        <v>-2.39</v>
+        <v>0</v>
       </c>
       <c r="H82" s="7" t="n">
-        <v>-2.39</v>
+        <v>1553.39</v>
       </c>
       <c r="I82" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J82" s="7" t="n">
-        <v>2.39</v>
+        <v>-1553.39</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B83" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D83" s="5" t="n">
-        <v>45196</v>
+        <v>45197</v>
       </c>
       <c r="E83" s="6" t="n">
-        <v>45197.75108796296</v>
+        <v>45197.403645833336</v>
       </c>
       <c r="F83" s="7" t="n">
-        <v>46.92</v>
+        <v>1677.89</v>
       </c>
       <c r="G83" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H83" s="7" t="n">
-        <v>46.92</v>
+        <v>1677.89</v>
       </c>
       <c r="I83" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J83" s="7" t="n">
-        <v>-46.92</v>
+        <v>-1677.89</v>
       </c>
       <c r="K83" s="3" t="s">
         <v>13</v>
@@ -3109,28 +3125,28 @@
         <v>1</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D84" s="5" t="n">
-        <v>45196</v>
+        <v>45198</v>
       </c>
       <c r="E84" s="6" t="n">
-        <v>45197.75108796296</v>
+        <v>45199.66027777778</v>
       </c>
       <c r="F84" s="7" t="n">
-        <v>2746.16</v>
+        <v>599.68</v>
       </c>
       <c r="G84" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H84" s="7" t="n">
-        <v>2746.16</v>
+        <v>599.68</v>
       </c>
       <c r="I84" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J84" s="7" t="n">
-        <v>-2746.16</v>
+        <v>-599.68</v>
       </c>
       <c r="K84" s="3" t="s">
         <v>13</v>
@@ -3138,34 +3154,34 @@
     </row>
     <row r="85" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B85" s="4" t="n">
-        <v>748</v>
+        <v>1</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D85" s="5" t="n">
-        <v>45196</v>
+        <v>45198</v>
       </c>
       <c r="E85" s="6" t="n">
-        <v>45197.75108796296</v>
+        <v>45199.66027777778</v>
       </c>
       <c r="F85" s="7" t="n">
-        <v>13968.83</v>
+        <v>1931.29</v>
       </c>
       <c r="G85" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H85" s="7" t="n">
-        <v>13968.83</v>
+        <v>1931.29</v>
       </c>
       <c r="I85" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J85" s="7" t="n">
-        <v>-13968.83</v>
+        <v>-1931.29</v>
       </c>
       <c r="K85" s="3" t="s">
         <v>13</v>
@@ -3173,34 +3189,34 @@
     </row>
     <row r="86" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B86" s="4" t="n">
-        <v>1</v>
+        <v>748</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D86" s="5" t="n">
-        <v>45197</v>
+        <v>45198</v>
       </c>
       <c r="E86" s="6" t="n">
-        <v>45197.403645833336</v>
+        <v>45199.66027777778</v>
       </c>
       <c r="F86" s="7" t="n">
-        <v>1553.39</v>
+        <v>5440.69</v>
       </c>
       <c r="G86" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H86" s="7" t="n">
-        <v>1553.39</v>
+        <v>5440.69</v>
       </c>
       <c r="I86" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J86" s="7" t="n">
-        <v>-1553.39</v>
+        <v>-5440.69</v>
       </c>
       <c r="K86" s="3" t="s">
         <v>13</v>
@@ -3217,196 +3233,56 @@
         <v>17</v>
       </c>
       <c r="D87" s="5" t="n">
-        <v>45197</v>
+        <v>45199</v>
       </c>
       <c r="E87" s="6" t="n">
-        <v>45197.403645833336</v>
+        <v>45200.41237268518</v>
       </c>
       <c r="F87" s="7" t="n">
-        <v>1677.89</v>
+        <v>63.6</v>
       </c>
       <c r="G87" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H87" s="7" t="n">
-        <v>1677.89</v>
+        <v>63.6</v>
       </c>
       <c r="I87" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J87" s="7" t="n">
-        <v>-1677.89</v>
+        <v>-63.6</v>
       </c>
       <c r="K87" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B88" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D88" s="5" t="n">
-        <v>45198</v>
-      </c>
-      <c r="E88" s="6" t="n">
-        <v>45199.66027777778</v>
-      </c>
-      <c r="F88" s="7" t="n">
-        <v>599.68</v>
-      </c>
-      <c r="G88" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H88" s="7" t="n">
-        <v>599.68</v>
-      </c>
-      <c r="I88" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J88" s="7" t="n">
-        <v>-599.68</v>
-      </c>
-      <c r="K88" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B89" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D89" s="5" t="n">
-        <v>45198</v>
-      </c>
-      <c r="E89" s="6" t="n">
-        <v>45199.66027777778</v>
-      </c>
-      <c r="F89" s="7" t="n">
-        <v>1931.29</v>
-      </c>
-      <c r="G89" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H89" s="7" t="n">
-        <v>1931.29</v>
-      </c>
-      <c r="I89" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J89" s="7" t="n">
-        <v>-1931.29</v>
-      </c>
-      <c r="K89" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B90" s="4" t="n">
-        <v>748</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D90" s="5" t="n">
-        <v>45198</v>
-      </c>
-      <c r="E90" s="6" t="n">
-        <v>45199.66027777778</v>
-      </c>
-      <c r="F90" s="7" t="n">
-        <v>5440.69</v>
-      </c>
-      <c r="G90" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H90" s="7" t="n">
-        <v>5440.69</v>
-      </c>
-      <c r="I90" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J90" s="7" t="n">
-        <v>-5440.69</v>
-      </c>
-      <c r="K90" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B91" s="4" t="n">
-        <v>748</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D91" s="5" t="n">
-        <v>45199</v>
-      </c>
-      <c r="E91" s="6" t="n">
-        <v>45200.41237268518</v>
-      </c>
-      <c r="F91" s="7" t="n">
-        <v>63.6</v>
-      </c>
-      <c r="G91" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H91" s="7" t="n">
-        <v>63.6</v>
-      </c>
-      <c r="I91" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J91" s="7" t="n">
-        <v>-63.6</v>
-      </c>
-      <c r="K91" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s"/>
-      <c r="B92" s="2" t="s"/>
-      <c r="C92" s="1" t="s"/>
-      <c r="D92" s="1" t="s"/>
-      <c r="E92" s="1" t="s"/>
-      <c r="F92" s="2" t="s">
+      <c r="A88" s="1" t="s"/>
+      <c r="B88" s="2" t="s"/>
+      <c r="C88" s="1" t="s"/>
+      <c r="D88" s="1" t="s"/>
+      <c r="E88" s="1" t="s"/>
+      <c r="F88" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G92" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H92" s="2" t="s">
+      <c r="H88" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I92" s="2" t="s">
+      <c r="I88" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J92" s="2" t="s">
+      <c r="J88" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K92" s="1" t="s"/>
+      <c r="K88" s="1" t="s"/>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError sqref="A1:K92" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:K88" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Retirado as capturas de tela
</commit_message>
<xml_diff>
--- a/cypress/downloads/Conciliação Bancária .xlsx
+++ b/cypress/downloads/Conciliação Bancária .xlsx
@@ -215,13 +215,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="17.43" min="1" max="1" customWidth="1"/>
-    <col width="19.71" min="2" max="2" customWidth="1"/>
+    <col width="17.29" min="1" max="1" customWidth="1"/>
+    <col width="19.57" min="2" max="2" customWidth="1"/>
     <col width="17.29" min="3" max="3" customWidth="1"/>
-    <col width="17.71" min="4" max="4" customWidth="1"/>
+    <col width="17.57" min="4" max="4" customWidth="1"/>
     <col width="29.86" min="5" max="5" customWidth="1"/>
     <col width="21.29" min="6" max="6" customWidth="1"/>
-    <col width="20.57" min="7" max="7" customWidth="1"/>
+    <col width="20.43" min="7" max="7" customWidth="1"/>
     <col width="20.86" min="8" max="8" customWidth="1"/>
     <col width="22" min="9" max="9" customWidth="1"/>
     <col width="31.86" min="10" max="10" customWidth="1"/>

</xml_diff>

<commit_message>
Teste criado em conciliação bancaria
</commit_message>
<xml_diff>
--- a/cypress/downloads/Conciliação Bancária .xlsx
+++ b/cypress/downloads/Conciliação Bancária .xlsx
@@ -215,13 +215,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="17.43" min="1" max="1" customWidth="1"/>
-    <col width="19.71" min="2" max="2" customWidth="1"/>
+    <col width="17.29" min="1" max="1" customWidth="1"/>
+    <col width="19.57" min="2" max="2" customWidth="1"/>
     <col width="17.29" min="3" max="3" customWidth="1"/>
-    <col width="17.71" min="4" max="4" customWidth="1"/>
+    <col width="17.57" min="4" max="4" customWidth="1"/>
     <col width="29.86" min="5" max="5" customWidth="1"/>
     <col width="21.29" min="6" max="6" customWidth="1"/>
-    <col width="20.57" min="7" max="7" customWidth="1"/>
+    <col width="20.43" min="7" max="7" customWidth="1"/>
     <col width="20.86" min="8" max="8" customWidth="1"/>
     <col width="22" min="9" max="9" customWidth="1"/>
     <col width="31.86" min="10" max="10" customWidth="1"/>

</xml_diff>